<commit_message>
redrafted to end of data cleaning section
</commit_message>
<xml_diff>
--- a/demo2.xlsx
+++ b/demo2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scottish-my.sharepoint.com/personal/brendan_clarke2_nes_scot_nhs_uk/Documents/projects/Dynamic report demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{80CE0118-CFC0-4FFB-857F-72C81A1B52E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{951068C8-7B5C-46FF-A8C9-D443644EDD70}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{80CE0118-CFC0-4FFB-857F-72C81A1B52E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CFD22279-38D2-4613-9D1E-DE92667FD88E}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1845" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -887,15 +887,15 @@
   <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -909,7 +909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44682</v>
       </c>
@@ -923,7 +923,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44683</v>
       </c>
@@ -937,7 +937,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44684</v>
       </c>
@@ -951,7 +951,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44685</v>
       </c>
@@ -965,7 +965,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44686</v>
       </c>
@@ -979,7 +979,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44687</v>
       </c>
@@ -993,7 +993,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44688</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44689</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44690</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44691</v>
       </c>
@@ -1049,12 +1049,12 @@
         <v>236</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44692</v>
       </c>
       <c r="B12">
-        <v>444</v>
+        <v>224</v>
       </c>
       <c r="C12">
         <v>980</v>
@@ -1063,7 +1063,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44693</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44694</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44695</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44696</v>
       </c>
@@ -1113,13 +1113,13 @@
         <v>96</v>
       </c>
       <c r="C16">
-        <v>660</v>
+        <v>8</v>
       </c>
       <c r="D16">
         <v>564</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44697</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44698</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44699</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44700</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44701</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44702</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44703</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44704</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44705</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44706</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44707</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44708</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44709</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44710</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44711</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44712</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44713</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44714</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44715</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44716</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44717</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44718</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44719</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44720</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44721</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44722</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44723</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44724</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44725</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44726</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44727</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44728</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44729</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44730</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44731</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44732</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44733</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44734</v>
       </c>
@@ -1645,13 +1645,13 @@
         <v>420</v>
       </c>
       <c r="C54">
-        <v>684</v>
+        <v>84</v>
       </c>
       <c r="D54">
         <v>264</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44735</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44736</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44737</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44738</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44739</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44740</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44741</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44742</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44743</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44744</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44745</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44746</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44747</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44748</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44749</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <f>A69+1</f>
         <v>44750</v>
@@ -1878,7 +1878,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <f t="shared" ref="A71:A86" si="0">A70+1</f>
         <v>44751</v>
@@ -1895,7 +1895,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <f t="shared" si="0"/>
         <v>44752</v>
@@ -1912,7 +1912,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <f t="shared" si="0"/>
         <v>44753</v>
@@ -1929,7 +1929,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <f t="shared" si="0"/>
         <v>44754</v>
@@ -1946,7 +1946,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <f t="shared" si="0"/>
         <v>44755</v>
@@ -1963,7 +1963,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <f t="shared" si="0"/>
         <v>44756</v>
@@ -1980,7 +1980,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <f t="shared" si="0"/>
         <v>44757</v>
@@ -1997,7 +1997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <f t="shared" si="0"/>
         <v>44758</v>
@@ -2014,7 +2014,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <f t="shared" si="0"/>
         <v>44759</v>
@@ -2031,7 +2031,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <f t="shared" si="0"/>
         <v>44760</v>
@@ -2048,7 +2048,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <f t="shared" si="0"/>
         <v>44761</v>
@@ -2065,7 +2065,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <f t="shared" si="0"/>
         <v>44762</v>
@@ -2082,7 +2082,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <f t="shared" si="0"/>
         <v>44763</v>
@@ -2099,7 +2099,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <f t="shared" si="0"/>
         <v>44764</v>
@@ -2116,7 +2116,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <f t="shared" si="0"/>
         <v>44765</v>
@@ -2133,7 +2133,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <f t="shared" si="0"/>
         <v>44766</v>

</xml_diff>